<commit_message>
Incomplete svc model added
</commit_message>
<xml_diff>
--- a/report/models_comparison.xlsx
+++ b/report/models_comparison.xlsx
@@ -52,13 +52,13 @@
     <t>logistic_regression</t>
   </si>
   <si>
+    <t>naive bayes</t>
+  </si>
+  <si>
+    <t>linear_svc</t>
+  </si>
+  <si>
     <t>perceptron</t>
-  </si>
-  <si>
-    <t>naive bayes</t>
-  </si>
-  <si>
-    <t>linear_svc</t>
   </si>
 </sst>
 </file>
@@ -450,19 +450,19 @@
         <v>0.95</v>
       </c>
       <c r="C2">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0.01</v>
       </c>
       <c r="F2">
-        <v>0.580927883435321</v>
+        <v>0.5607830844417628</v>
       </c>
       <c r="G2">
-        <v>0.580927883435321</v>
+        <v>0.5607830844417628</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -476,16 +476,16 @@
         <v>0.54</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0.01</v>
       </c>
       <c r="F3">
-        <v>0.5406491526509868</v>
+        <v>0.53677130971461</v>
       </c>
       <c r="G3">
-        <v>0.5406491526509868</v>
+        <v>0.53677130971461</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -505,10 +505,10 @@
         <v>0.01</v>
       </c>
       <c r="F4">
-        <v>0.5290247425878398</v>
+        <v>0.5336433037701915</v>
       </c>
       <c r="G4">
-        <v>0.5290247425878398</v>
+        <v>0.5336433037701915</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -516,7 +516,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="C5">
         <v>0.46</v>
@@ -525,13 +525,13 @@
         <v>0.02</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F5">
-        <v>0.4617000370940548</v>
+        <v>0.4586203688691701</v>
       </c>
       <c r="G5">
-        <v>0.4617000370940548</v>
+        <v>0.4586203688691701</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -539,10 +539,10 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.8</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C6">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="D6">
         <v>0.01</v>
@@ -551,10 +551,10 @@
         <v>0.02</v>
       </c>
       <c r="F6">
-        <v>0.4408248851079835</v>
+        <v>0.4454779218428099</v>
       </c>
       <c r="G6">
-        <v>0.4408248851079835</v>
+        <v>0.4454779218428099</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -565,19 +565,19 @@
         <v>0.62</v>
       </c>
       <c r="C7">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="D7">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E7">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F7">
-        <v>0.3833788517708521</v>
+        <v>0.385767260489444</v>
       </c>
       <c r="G7">
-        <v>0.3833788517708521</v>
+        <v>0.385767260489444</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -585,22 +585,22 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.44</v>
+        <v>0.52</v>
       </c>
       <c r="C8">
         <v>0.37</v>
       </c>
       <c r="D8">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E8">
         <v>0.02</v>
       </c>
       <c r="F8">
-        <v>0.3718399989693308</v>
+        <v>0.3702680024541976</v>
       </c>
       <c r="G8">
-        <v>0.3718399989693308</v>
+        <v>0.3702680024541976</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -608,22 +608,22 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.61</v>
       </c>
       <c r="C9">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="D9">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E9">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F9">
-        <v>0.3733005794670268</v>
+        <v>0.3563253812848866</v>
       </c>
       <c r="G9">
-        <v>0.3733005794670268</v>
+        <v>0.3563253812848866</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -631,22 +631,22 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.6</v>
+        <v>0.49</v>
       </c>
       <c r="C10">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="D10">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E10">
         <v>0.01</v>
       </c>
       <c r="F10">
-        <v>0.3485911788430369</v>
+        <v>0.3563268787670251</v>
       </c>
       <c r="G10">
-        <v>0.3485911788430369</v>
+        <v>0.3563268787670251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>